<commit_message>
one more set of numbers to show it seems to not matter very much what the answer is
</commit_message>
<xml_diff>
--- a/execution/RetroPE/DJ.xlsx
+++ b/execution/RetroPE/DJ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carette/research-repos/Theseus/execution/RetroPE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8103ED81-5E52-D84F-979D-9371C491B3C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2986244-035D-864D-9881-325F46CE33C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10240" yWindow="1000" windowWidth="18180" windowHeight="16440" xr2:uid="{7955564F-C61D-284E-9FC7-8ED54B9D9B74}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>kind</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>bal1</t>
+  </si>
+  <si>
+    <t>bal4</t>
   </si>
 </sst>
 </file>
@@ -408,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46C075C9-91FC-154A-9140-631FCC6663F8}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -535,6 +538,57 @@
         <v>60.25</v>
       </c>
     </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>10</v>
+      </c>
+      <c r="D14">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C15">
+        <v>11</v>
+      </c>
+      <c r="D15">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C16">
+        <v>12</v>
+      </c>
+      <c r="D16">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C17">
+        <v>13</v>
+      </c>
+      <c r="D17">
+        <v>2.52</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C18">
+        <v>14</v>
+      </c>
+      <c r="D18">
+        <v>11.39</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C19">
+        <v>15</v>
+      </c>
+      <c r="D19">
+        <v>54.75</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>